<commit_message>
added streamlit app created mongo db and sqlite database
</commit_message>
<xml_diff>
--- a/files/data.xlsx
+++ b/files/data.xlsx
@@ -458,426 +458,214 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/71830889?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Старший клиентский менеджер (с. Петровское)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>от 34600 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Сбер — лучший работодатель России. У нас более 60 компаний экосистемы и 14 тысяч подразделений по всей стране. Мы ищем старшего менеджера по сопровождению клиентов. Его главная задача – помогать клиентам с оформлением продуктов и услуг Сбера и экосистемы, а также консультировать по возникающим вопросам. Эта вакансия для тех, кто хочет развивать навыки эффективных продаж и стоить карьеру в банковской сфере. Эта работа подойдет тебе если ты: · специалист со средним профессиональным, неполным высшим или высшим образованием · имеешь опыт работы в сфере продаж, обслуживания и консультирования клиентов от 6 месяцев · доброжелателен и готов помогать клиентам.   Тебе предстоит:   · предлагать продукты и услуги Сбера · консультировать клиентов по возникающим вопросам · помогать клиентам оформлять услуги и необходимые для них документы · совершать транзакционные операции в рамках оформления продаж и постпродажного сопровождения клиентов · вести базы клиентов.   Работа в Сбере – это:  · стабильный оклад и социальная поддержка сотрудников · официальное оформление с первого дня · расширенный ДМС с первого дня и льготное страхование для близких · корпоративное обучение в Виртуальной школе Сбера · бесплатная подписка СберПрайм+, скидки на продукты компаний-партнеров · корпоративная пенсионная программа · ипотека выгоднее на 4% для каждого сотрудника.   Присоединяйся к команде старших клиентских менеджеров Сбера!АтмосфераРабота в Сбере – это:Обучение за счет компании: онлайн курсы в Виртуальной школе Сбера, возможность получить новую квалификациюРеферальная программа для сотрудников: пригласи в команду знакомых профессионалов и получи свое вознагр</t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76330761?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/45158261?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Водитель категории Е</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>от 82000 до 110000 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Мы повысили заработную плату !!!!!!!!!! Логистика – одно из главных направлений в компании «Магнит». Уже более четверти века у нас всё в порядке!   Работа с нами — это:    достойная своевременная зарплата, два раза в месяц. платим гарантированный оклад плюс премию: влияй на свой доход! удобный график: 4/2, 5/5, 6/3 , 4/4 курсы безопасного и экономичного вождения за наш счёт. собственные ремзоны на каждом АТП. вводим в курс дела, даём наставника. бесплатные медосмотры. оформление карт тахографа за счёт компании. выплаты за экономию топлива. акция «Приведи друга» - возможность дополнительного заработка. возможность проявить себя: участвуй в конкурсах профессионального мастерства! полное соблюдение требований ТК РФ    Комфортные условия труда:    удобная спецодежда и защитная обувь. Комплекты для зимы: два вида тёплых курток и обуви (для суровых заморозков и на время оттепели), комбинезон и перчатки. На лет</t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76331077?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/45158696?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Водитель категории Е (транзитная доставка)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>до 115000 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Мы повысили заработную плату !!!!!!!!!! Логистика – одно из главных направлений в компании «Магнит». Уже более четверти века у нас всё в порядке! Работа с нами — это:  достойная своевременная зарплата, два раза в месяц. платим гарантированный оклад плюс премию: влияй на свой доход! удобный график: 20/10, 25/5, 28/14, 30/15 курсы безопасного и экономичного вождения за наш счёт. собственные ремзоны на каждом АТП. вводим в курс дела, даём наставника. бесплатные медосмотры. оформление карт тахографа за счёт компании. выплаты за экономию топлива. акция «Приведи друга» - возможность дополнительного заработка. возможность проявить себя: участвуй в конкурсах профессионального мастерства! полное соблюдение требований ТК РФ    Комфортные условия труда:    удобная спецодежда и защитная обувь. Комплекты для зимы: два вида тёплых курток и обуви (для суровых заморозков и на время оттепели), комбинезон и перчатки. На лето – комбинезон, куртка, обувь, перчатки. корпоративная связь. выдаём планшеты с корпоративной связью для помощи в пути. оказываем оперативную помощь на дорогах. возможно проживание на территории в комнате отдыха для водителей    Обязанности. Что нужно делать?    доставлять товары на автомобилях MAN. С нас: ремонт автомобиля и чёткие задачи. ценить машину как свою.    Требования.    нам неважно, какой у тебя официальный стаж работы, мы ценим и развиваем талантливых водителей.    Достаточно стать частью логистики «Магнита», чтобы…    всё было в порядке. найти крепкую и надёжную команду. обеспечить свое материальное благополучие. работать в компании – мировом лидере по эксплуатации MAN. стать частью самой крупной логистической компании в стране: более 39 тысяч. сотрудников, порядка 5,5 тысяч грузовиков, 39 распределительных центров и 37 автотранспортных предприятий. Стань частью семьи «Магнит»!АО "Тандер" представляет бренд МагнитЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбовская область, Тамбовский район, ул. Комплекс Мотель, д. 2Показать на большой к</t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76153963?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/72339200?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Менеджер по работе с ключевыми клиентами малого бизнеса</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>от 58000 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">  Сбер — лучший работодатель России. У нас более 60 компаний экосистемы и 14 тысяч подразделений по всей стране. Присоединяйся к команде малого бизнеса Сбера! На позиции «Менеджера по работе с ключевыми клиентами» ты будешь общаться с предпринимателями и руководителями компаний малого бизнеса и предлагать лучшие решения от Сбера. Эта вакансия для энергичных и общительных людей, готовых вникать в тонкости бизнеса наших клиентов. Мы поможем тебе освоить специальность, сформируем для тебя базу клиентов, предоставим возможности карьерного роста. Тебе предстоит:  развивать бизнес клиентов из закрепленной базы, предлагая продукты и услуги Сбера проводить переговоры с клиентами на территории компаний-партнеров привлекать новых клиентов на обслуживание в Сбер проводить переговоры с предпринимателями и руководителями компаний выстраивать долгосрочное сотрудн</t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76330670?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/71831503?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Старший менеджер по обслуживанию (с. Покрово-Марфино)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>от 9600 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Сбер — это 14 тысяч подразделений и лучший работодатель России по версии hh.   Старшие менеджеры по обслуживанию в Сбере – это специалисты, которые проводят операции клиентов в кассе: помогают обменивать деньги, принимают и выдают наличные.   Эта работа подойдет тебе если ты:   · ищешь работу на неполный день или дополнительный заработок к основной работе · хочешь построить карьеру в банковской сфере · ищешь работу с возможностью карьерного перемещения по всей стране · специалист со средним профессиональным, неполным высшим или высшим образованием · хочешь работать в надежной компании · имеешь опыт работы в сфере продаж, обслуживания и консультирования клиентов от полугода.   Тебе предстоит:   · работать в отделении офиса Сбера · проводить кассовые операции: прием, выдача, обмен денег · предлагать продукты и сервисы Сбера · консультировать клиентов по возникающим вопросам.   Работа в Сбере – это:   · стабильный оклад и социальная поддержка сотрудников · возможность выбрать удобный график работы · дополнительный доход ежемесячно · возможностью совмещать работу с другой занятостью и увлечениями · официальное оформление · расширенная пенсионная программа · бесплатная подписка СберПрайм+ и скидки на продукты компаний-партнеров · оплачиваемая мобильная связь: 150 минут и 3 ГБ интернета Сбермобайла · ипотека выгоднее на 4%.   Присоединяйся к команде Сбера!    АтмосфераРабота в Сбере – это:Обучение за счет компании: онлайн курсы в Виртуальной школе Сбера, возможность получить новую квалификациюРеферальная программа для сотрудников: пригласи в команду знакомых профессионалов и получи свое вознаграждение до 100 тыс. рублейКурсы для будущих родителей, материальная поддержка молодых мам, детский отдых и подарки за счет компанииКорпоративная пенсионная программаДелай мир лучше со СберомЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресПокрово-МарфиноПоказать на большой карте</t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76330136?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75849751?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Документовед</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>от 18000 до 25000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Требования к умениям:- работать на компьютере, в том числе в сети Интернет;- работать в информационно-правовых системах.Функции:Ведение делопроизводства комитета.Ведение кадрового делопроизводства в комитете.Задайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, Коммунальная улица, 6Показать на большой карте</t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76330688?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75833387?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Junior Python Developer</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>от 35000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>AstraLab - одна из самых инновационных компаний российского рекламного рынка. Мы первые в России и четвертые в мире научились интегрировать рекламу в фото на базе компьютерного зрения. У нас есть собственная технология AstraVision: компьютерное зрение + обработка языка и текстов. Мы также сотрудничаем с крупнейшим селлером рекламы в стране - ИМХО. С 2018 года мы работаем с клиентами по всему миру и сотрудничаем с крупнейшими сетевыми агентствами (GroupM, BBDO, Dentsu Aegis Network, Publicis Groupe) и брендами (Audi, Lexus, Honda, Pepsi, Nestle, Red Bull, Asus, P&amp;G, Schwarzkopf и др.) Компания Astralab ищет Junior Python разработчика для помощи в создании инновационных программных решений. Мы ищем начинающего разработчика с опытом использования языка Python и желанием научиться чему-то новому. Кандидат должен иметь общее понимание основ программирования и хорошие коммуникационные навыки. Опыт работы с базами данных и системами контроля версий также будет приветствоваться. Эта вакансия предлагает занятость на полный рабочий день в нашем офисе в городе Тамбов. Мы предлагаем конкурентный оклад и перспективы карьерного роста. Обязанности:  Разработка и поддержка backend приложений на Python (Fast API). Разработка нового функционала и сервисов. Интеграция со сторонними сервисами по API. Участвовать в разработке продуктов нашей компании. Решать технические вопросы и помогать в поддержке продуктов. Постоянно совершенствовать свои навыки и знания в области разработки на Python.  Ожидания:  Наличие опыта в разработке на языке Python. Наличие общих знаний в области программирования и опыта работы в команде разработчиков. Желание учиться и развиваться в области разработки на Python. Творческий подход и инициатива в решении технических задач. Умение общаться и эффективно сотрудничать с другими членами команды. Знание алгоритмов и структур данных.  **Плюсом будет ***:  Базовое понимание основ ML и Computer Vision. Умение разбираться в чужом коде. Инициативность и приверженность к самосовершенствованию.  При отсутствии опыта, научим. Условия работы:  Дружная молодая команда и лёгкая коммуникация: мы не придерж</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Python / Git / Базы данных / REST API / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76153964?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75913933?from=vacancy_search_list</t>
+          <t>https://hh.ru/vacancy/73003608?from=vacancy_search_list</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Сектетарь</t>
+          <t>Водитель-экспедитор, г. Тамбов</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>до 23514 руб. до вычета налогов</t>
+          <t>от 51000 до 54000 руб. до вычета налогов</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Описание работодателя: ТОГУП "Водное и газовое хозяйство" приглашает на работу секретаря Опыт работы приветствуется. График 5/2 с 08:00 до 17:00. Обязанности:  прием входящей корреспонденции, подготовка документов на подпись руководителю, распределение документооборота, контроль за сроками исполнения поручений руководителя. Требования:  базовые знания офисных программ, ответственность, внимательность, грамотность, дисциплинированность  Задайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, Студенецкая улица, 3Показать на большой карте</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr"/>
+          <t>Обязанности:  Доставка, экспедирование грузов по городу, области Оформление путевой и транспортной документации  Требования:  Образование от среднего Опыт работы от 3-х лет Наличие прав категории В Знание устройства автомобилей Исполнительность, умение работать в команде, готовность к принятию решений  Условия:  Ненормированный рабочий день, график работы сменный з/п от 51 000 до 54 000 руб. Трудоустройство в соответствии с ТК РФ, полный соц.пакет подарки для детей сотрудников Компенсация питания Доставка до места работы Дополнительные льготы сотрудникам Ключевые навыкиПользователь ПКРабота в командеГрамотная речьВодительское удостоверение категории Bоформление документацииУсловия для водителей Нужны права категории B;  Военный билет не нужен.Категория BПеревозка грузо</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Пользователь ПК / Работа в команде / Грамотная речь / Водительское удостоверение категории B / оформление документации / </t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/74190112?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Помощник руководителя</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>от 50000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Обязанности:  прием входящих звонков, организация приема посетителей, прием документов на подпись руководителю, организация совещаний, выполнение личных и служебных поручений руководителя.  Требования:  высшее образование, опыт аналогичной работы от 1 года, грамотная речь, уверенный пользователь ПК, вежливость, доброжелательность, исполнительность, пунктуальность.  Условия:  пятидневная рабочая неделя (выходные - суббота, воскресенье), оформление по ТК РФ. Ключевые навыкиОрганизация мероприятийПрием посетителейПрием и распределение звонковДеловая корреспонденцияРабота с первыми лицами компанииДокументооборотКоммуникабельностьАнглийский — B1 — СреднийЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, Моршанское шоссе, 36Показать на большой карте</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Организация мероприятий / Прием посетителей / Прием и распределение звонков / Деловая корреспонденция / Работа с первыми лицами компании / Документооборот / Коммуникабельность / Английский — B1 — Средний / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76330138?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75912279?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Секретарь-делопроизводитель/ведущий специалист общего отдела</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>от 32000 до 35000 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>В муниципальное казенное учреждение, сферой деятельности которого является организация капитального строительства, реконструкции, капитального и текущего ремонта объектов жилищно-коммунального назначения, социальной, производственной и инженерной инфраструктуры города Тамбова, требуется ведущий специалист общего отдела. График работы – 5-ти дневная рабочая неделя; суббота, воскресенье - выходной; Опыт работы – не менее 3 лет ; Требования: высшее образование; Обязанности: Выполнение технических функций по обеспечению и обслуживанию работы директора учреждения и его заместителей (организовывать телефонные переговоры директора и подразделений учреждения, передавать телефонограммы, осуществлять работу по подготовке совещаний, вести протоколы совещаний, передавать и принимать информацию по телефону, факсу и др.); - ведение делопроизводства (принимать поступающу</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Делопроизводство / Организаторские навыки / Кадровое делопроизводство / Деловая переписка / Внутренняя документация / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76154582?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75838301?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Водитель автомобиля</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>от 30000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Обязанности:  Управление автомобилем Проверка технического состояния и прием автомобиля перед выездом, сдача его и постановка на отведенное место по возвращении на предприятие; Заправка автомобиля топливом, смазочными материалами. Подача автомобиля под погрузку и разгрузку грузов и контроль за погрузкой; Оформление путевых документов.  Требования:  Права категории В, С.  Условия:  Трудоустройство согласно ТК РФ. Ключевые навыкиВодительское удостоверение категории Bоформление документацииУмение работать в командеЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, Моршанское шоссе, 21Показать на большой карте</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Водительское удостоверение категории B / оформление документации / Умение работать в команде / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76153877?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75826196?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Секретарь учебной части</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>от 17000 до 17000 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Обязанности:   оформляет личные дела принятых на обучение и протоколы приемной комиссии колледжа;   оформляет зачетные книжки, студенческие билеты обучающихся, экзаменационные ведомости;   ведет учет часов учебной работы преподавателей и посещаемости занятий обучающихся;   готовит журналы учебных занятий, приказы и распоряжения по движению контингента обучающихся;   оформляет протоколы заседаний предметно-цикловых комиссий;   Требования:   среднее профессиональное или высшее образование в области делопроизводства;   уверенный пользователь ПК;   владение офисными пакетами «Мой офис» и LibreOffice;   владение оргтехникой;   Условия:   постоянная работа;   понедельник-пятница с 09:00 до 18:00;   стабильная заработная плата;   Оформление по ТК РФ;   2 класс условий труда  Ключевые навыкиПользователь ПКДелопроизводствоРабота с оргтехникойOpenOfficeоформление документацииОфисные программыLibreOfficeЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, улица Августа Бебеля, 21Показать на большой карте</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Пользователь ПК / Делопроизводство / Работа с оргтехникой / OpenOffice / оформление документации / Офисные программы / LibreOffice / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76153959?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75832579?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Junior Frontend Developer (Vue.js)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>от 35000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>AstraLab - одна из самых инновационных компаний российского рекламного рынка. Мы первые в России и четвертые в мире научились интегрировать рекламу в фото на базе компьютерного зрения. У нас есть собственная технология AstraVision: компьютерное зрение + обработка языка и текстов. Мы также сотрудничаем с крупнейшим селлером рекламы в стране - ИМХО. С 2018 года мы работаем с клиентами по всему миру и сотрудничаем с крупнейшими сетевыми агентствами (GroupM, BBDO, Dentsu Aegis Network, Publicis Groupe) и брендами (Audi, Lexus, Honda, Pepsi, Nestle, Red Bull, Asus, P&amp;G, Schwarzkopf и др.) Компания Astralab ищет амбициозного Frontend разработчика, который хочет принять участие в создании уникальных и инновационных продуктов. Если вы любите работать с современными технологиями и инструментами, и хотите развиваться в компании с динамичным ростом и высокими стандартами качества, то эта вакансия для вас. Обязанности  Разработка веб-приложений; Оптимизация и модернизация существующих решений; Проведение тестирования; Решение технических вопросов по интеграции продуктов.  Ожидания  Знания JavaScript; Опыт работы с vue.js (vuex, vue router); Знание основных принципов ООП и шаблонов проектирования; Знание HTML5, CSS3, семантическая разметка; Умение работы с веб-шрифтами; Опыт работы с Git.  Плюсом будет  Использование CSS препроцессоров (SASS / LESS / Stylus / PostCSS) или CSS Modules; Использование инструментов линтинга (eslint) и форматинга (prettier). Умение их настраивать и понимание принципов работы; Опыт работы с высоконагруженными проектами; Опыт работы со сборщиками проектов (Webpack, Gulp).  Условия  Дружная молодая команда и лёгкая коммуникация: мы не придерживаемся иерархии в управлении продуктом, ценим открытое командное взаимодействие, общаемся и дружим вне работы. Интересные задачи в передовых продуктах: наши продукты являются передовыми на рынке, поэтому перед командой разработки часто ставятся сложные задачи, требующие неординарного подхода. Акцент на качестве кода и производительности: мы считаем, что залог эффективности продукта — качественный код, поэтому используем методику гибкого код ревью. Профессиональный рост и реализация идей: мы поощряем инициативу в команде и помогаем в развитии навыков и идей. Удобный график в офисе: с понедельника по пятницу, гибкие начало и окончание рабочего дня. Оформление: мы соблюдаем трудовое законодательство, официально оформляем на работу и предоставляем все гарантии по ТК РФ (отпуск, больничные и т.п.)     Ключевые навыкиJavaScriptHTML5CSS3Vue.jsЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопрос</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">JavaScript / HTML5 / CSS3 / Vue.js / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76154580?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75527075?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Персональный водитель</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>от 45000 до 45000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Обязанности: -Обеспечение комфортного сопровождения на автомобиле руководителя-Выполнение различных поручений руководителя-Подача автомобиля в назначенное место и время-Осуществление контроля за техническим состоянием автомобиля-Уход за автомобилем, содержание его в чистоте-Соблюдение водительского этикета   Требования:-Профессиональный опыт вождения не менее 5 лет-Отличное знание дорог города Тамбова и Тамбовской области-Готовность к ненормированному рабочему дню-Опыт работы персональным водителем на машинах представительского класса ОБЯЗАТЕЛЕН   Условия:-График работы ненормированный-Оформление по ТК РФ, заработная плата по итогам собеседования.Ключевые навыкиВождение автомобилей представительского классаЗнание устройства автомобиляИсполнение личных поручений руководителяВодительское удостоверение категории BЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопрос</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Вождение автомобилей представительского класса / Знание устройства автомобиля / Исполнение личных поручений руководителя / Водительское удостоверение категории B / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76330133?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+      <c r="E15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75846268?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Управляющий по открытию и дальнейшему управлению торговой точкой</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>от 50000 руб. на руки</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>ГК ТМК имеет 20-летний опыт производства и продажи окон, входных и межкомнатных Дверей, а также сопутствующих товаров. На данный момент наши офисы есть почти в каждом регионе ЦФО. 200 офисов продаж и 2000 довольных сотрудников Мы ищем в свою команду Управляющего для открытия и дальнейшего управления торговой точки (300-500 м2). Обязанности:   выбор локации под открытие торговой точки;   управление операционной деятельностью торговой точки;   работа с персоналом: подбор, адаптация, обучение и мотивация сотрудников;   контроль качества обслуживания, обеспечение трудовой дисциплины;   выполнение плановых показателей по продажам торговой точки;   исполнение стандартов работы с клиентами и соблюдения технологии продаж;   разработка мероприятий по привлечению клиентов;   подбор, обучение менеджеров активных продаж, постановка планов и контроль их выполнения;   проведение мониторинга конкурентов;   контроль кассовой дисциплины.   Требования:  опыт в открытии торговых точек;  успешный опыт руководства коллективом и построения команды с нуля;   энергичность, позитивность, ориентирование на результат, а не на процесс;   высокоразвитые коммуникативные навыки и клиентоориентированность;   успешный опыт личных продаж;   готовность участвовать во всех процессах в продажах, глубоко погружаться в нюансы;   у</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Управление персоналом / Навыки продаж / Прямые продажи / 1С: Торговля / Обучение и развитие / Руководство коллективом / 1С: Предприятие: Розница / Умение принимать решения / Мотивация / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76331061?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+      <c r="E16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75831466?from=vacancy_search_list</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Водитель персональный</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>от 18000 до 30000 руб. до вычета налогов</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Обязанности:  Персональный водитель  Требования:  Аккуратный  Условия:  Стабильное учреждение Хороший коллектив Комфортное место для отдыха в перерыве от работы Премии Ключевые навыкиРабота в командеГрамотная речьУмение работать в коллективеОтветственность и пунктуальностьЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, Советская улица, 106АПоказать на большой карте</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Работа в команде / Грамотная речь / Умение работать в коллективе / Ответственность и пунктуальность / </t>
-        </is>
-      </c>
+          <t>https://hh.ru/vacancy/76153876?from=vacancy_search_list</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+      <c r="E17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75536473?from=vacancy_search_list</t>
+          <t>https://hh.ru/vacancy/73871478?from=vacancy_search_list</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Сотрудник в полиграфию</t>
+          <t>Старший менеджер по обслуживанию</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>от 25000 до 40000 руб. на руки</t>
+          <t>от 30900 руб. до вычета налогов</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>У нас полный цикл производства сувенирной продукции. Еженедельно отгружаемся на Wildberries и Ozon. Много ручной работы - сборка, сортировка, накрутка, упаковка. Требуется скорость, аккуратность и внимательность. Есть склад - надо понимать, что, где лежит и в каком количестве. Всё фиксируется в простых эксельках - будет плюсом, если вы шарите в табличках и любите порядок и структуру. Научим формироваь поставки на ВБ и Озон. Пару раз в неделю надо будет сделать отгрузку в траспортную компанию или отъехать по рабочим вопросам. Поэтому наличие своей машины обязательно. Бензин оплачивается. При желании можем научить работать на оборудовании и в принципе погрузить целиком в процесс, если будет интересно развиваться и расти в зарплате. У нас небольшой коллектив, комфортное для работы помещение в районе Ашана. Зимой тепло, летом прохладно, чай/кофе и печеньки. Зарплата каждую неделю без задержек. Оплачиваемая стажировка. График с 9ти до 18ти с перерывом на обед. Среда и воскресенье выходные.Задайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, Советская улица, 189БПоказать на большой карте</t>
+          <t>Сбер — лучший работодатель России. У нас более 60 компаний экосистемы и 14 тысяч подразделений по всей стране. Мы ищем старших менеджеров по обслуживанию клиентов Сбера. Это специалисты, которые проводят операции клиентов отделения банка.   Эта работа подойдет тебе если ты: · хочешь стать экспертом в банковской сфере · доброжелателен и готов помогать клиентам · специалист со средним профессиональным, неполным высшим или высшим образованием · владеешь программами Microsoft Office, Outlook · готов к работе, предполагающей ежедневное проведение однотипных операций.   Тебе предстоит: · осуществлять операции по обслуживанию клиентов · проводить кассовые операции: прием, выдача, обмен денег · предлагать продукты и сервисы Сбера · консультировать клиентов по возникающим вопросам.     Работа в Сбере – это:  · стабильный оклад и социальная поддержка сотрудников · официальное оформление с первого дня · ДМС с первого дня и льготное страхование для близких · корпоративное обучение в Виртуальной школе Сбера · бесплатная подписка СберПрайм+, скидки на продукты компаний-партнеров · корпоративная пенсионная программа · ипотека выгоднее на 4% для каждого сотрудника.     Присоединяйся к команде старших менеджеров по обслуживанию Сбера!  АтмосфераРабота в Сбере – это:Обучение за счет компан</t>
         </is>
       </c>
       <c r="E18" t="inlineStr"/>
@@ -885,83 +673,75 @@
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75834762?from=vacancy_search_list</t>
+          <t>https://hh.ru/vacancy/76114455?from=vacancy_search_list</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Специалист по кадрам</t>
+          <t>Старший специалист по продажам корпоративным клиентам (b2b)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>от 27000 до 27000 руб. на руки</t>
+          <t>от 50000 руб. до вычета налогов</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Обязанности:  Ведение кадрового делопроизводства в полном объеме - 50 чел. Ведение воинского учета; Работа с персональными данными; Ведение штатного расписания, составление, изменение; Подготовка справок, копий трудовых книжек и др. документов с места работы по запросу работников, в т.ч. для работников, выходящих на пенсию по возрасту и досрочно; Ведение табеля учета рабочего времени Подготовка и сдача отчетности: в СФР, сведения в службу занятости населения, в Росстат; Консультация руководства и специалистов учреждения по вопросам, касающихся трудового законодательства; Отчётность с использованием программы Контур-Экстерн. Прием документов и личных заявлений на подпись директору, составление писем, запросов, других документов, подготовка ответов авторам писем по поручению директора. Ведение отдельных служебных поручений директора; Доведение до сведения работников организационных, распорядительных и кадровых документов; Прием больничных листов;  Требования:  Желательно высшее образование, дополнительная подготовка по направлению; Опыт работы от 3-х лет по настоящее время в аналогичной должности по всем кадровым процессам; Отличное знание Трудового кодекса РФ, нормативных актов; Знание изменений и требований к отчетности, предъявляемые в настоящее время; Желание работать и развиваться в своей профессии; Усидчивость, внимательность, высокая степень ответственности, оперативность, скрупулёзность, стрессоустойчивость, коммуникабельность, честность и открытость; Грамотная устная и письменная речь.  Условия:  Оформление по ТК РФ, полный соц. пакет; График работы: 5/2, с 8:30 до 17:30 с перерывом на обед. Суббота и воскресенье - выходной день; Стабильная заработная плата, выплаты 2 раза в месяц. Ключевые навыкиПользователь ПККадровое делопроизводствоТрудовое законодательство РФУверенный пользователь ПКОтчетностьЗнание трудового законодательстваГрамотная устная и письменная речьТабель учета рабочего времениДеловая перепискаЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, улица Монтажников, 1Показать на большой карте</t>
+          <t>Билайн предоставляет услуги как крупнейшим международным компаниям, так и предприятиям среднего и малого бизнеса.Наша команда B2B всегда готова предложить клиентам самые современные технологии, от облачных АТС и мобильного CRM до продвинутых технологических решений на основе Big Data, облачные хранилища и многое другое. Итак, тебе предстоит:  Выполнять еженедельные минимальные требования по активности; Качественно отрабатывать ЛИДы от подразделения Telesales; Самостоятельно осуществлять поиск и привлечение новых клиентов ( базы и выгрузки предоставляются! ); Осуществлять допродажи клиентам малого и среднего бизнеса; Выявлять «скрытые» потребности клиентов; Развивать партнерские отношения, а так же осуществлять продажи на объектах коммерческой недвижимости; Формировать качественную воронку продаж; Выполнять личные KPI.  Мы будем рады рассмотреть твою кандидатуру, если у тебя есть:  Успешный опыт работы в сфере продаж от 1 года; Знание технологии и этапов продаж; Отличные презентационные и коммуникативные навыки.  Что мы предлагаем:  Работа в крупной и стабильной компании; Обучение и программа адаптации для новых сотрудников; Официальное оформление по ТК РФ + 2 дня дополнительно к ежегодному отпуску; Фиксированный оклад + ежемесячная премия (без потолка); График 5/2 (административный график/производственный календарь); Работа в современном офисе по адресу улица Коммунальная , 25.  В Билайн мы развиваем и поддерживаем здоровую и безопасную рабочую среду. Каждый сотрудник соблюдает Кодекс поведения, внутренние правила компании и придерживается принципов деловой этики. Мы поступаем честно и этично как по отношению друг к другу, так и к нашим внешним партнерам.Удаленная работаУчастие в конференцияхКорпоративная связьбилайн университетМедицинское страхованиеСкидки на изучение английскогоПАО "ВЫМПЕЛКОМ" представляет бренд билайнКлючевые навыкиB2B ПродажиВедение переговоровПланирование продажНавыки продажРазвитие ключе</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Пользователь ПК / Кадровое делопроизводство / Трудовое законодательство РФ / Уверенный пользователь ПК / Отчетность / Знание трудового законодательства / Грамотная устная и письменная речь / Табель учета рабочего времени / Деловая переписка / </t>
+          <t xml:space="preserve">B2B Продажи / Ведение переговоров / Планирование продаж / Навыки продаж / Развитие ключевых клиентов / Навыки презентации / Деловое общение / CRM / </t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75742131?from=vacancy_search_list</t>
+          <t>https://hh.ru/vacancy/71830892?from=vacancy_search_list</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Сотрудник пункта выдачи интернет заказов</t>
+          <t>Старший менеджер по обслуживанию (с. Малиновка)</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>от 15000 до 17000 руб. на руки</t>
+          <t>от 15500 руб. до вычета налогов</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Работа в OZON Менеджер в ПВЗ Тамбов, улица Киквидзе, 102 График работы: Два через два 09:00-20:00Размер заработной платы: 15 000 ₽Частота выплат: Дважды в месяцГде предстоит работать: Тамбов, улица Киквидзе, 102Опыт работы: Не имеет значенияЧто мы ждём:1) Пунктуальность. ПВЗ должен открываться вовремя, поэтому опаздывать работнику нельзя.2) Грамотная русская речь и доброжелательность.3) Внимательность, стрессоустойчивость, исполнительность, ответственность, умение избегать конфликтов.4) Умение работать на ПК и с оргтехникой.В чём заключается работа:1) Пpиём и соpтиpoвкa посылок на cклад2) Выдача заказов клиентам, приём возвратов3) Проведение инвентаризации4) Формирование возвратных перевозок5) Поддержка чистоты и порядка на рабочем месте6) Приём наличной/безналичной оплаты; работа с кассой.Условия для сотрудничества:1) Комфортный график для работы/подработки.2) Начинающим работникам всегда помогают внимательные наставники.3) Отдельное помещение для отдыха и приема пищи (кулер с питьевой водой, печь СВЧ).4) Всегда своевременная оплата.Ключевые навыкиГрамотная речьПользователь ПКРабота с оргтехникойРабота в командеРабота с клиентамиЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресТамбов, улица Киквидзе, 102Показать на большой карте</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Грамотная речь / Пользователь ПК / Работа с оргтехникой / Работа в команде / Работа с клиентами / </t>
-        </is>
-      </c>
+          <t>Сбер — это 14 тысяч подразделений и лучший работодатель России по версии hh.   Старшие менеджеры по обслуживанию в Сбере – это специалисты, которые проводят операции клиентов в кассе: помогают обменивать деньги, принимают и выдают наличные.   Эта работа подойдет тебе если ты:   · ищешь работу на неполный день или дополнительный заработок к основной работе · хочешь построить карьеру в банковской сфере · ищешь работу с возможностью карьерного перемещения по всей стране · специалист со средним профессиональным, неполным высшим или высшим образованием · хочешь работать в надежной компании · имеешь опыт работы в сфере продаж, обслуживания и консультирования клиентов от полугода.   Тебе предстоит:   · работать в отделении офиса Сбера · проводить кассовые операции: прием, выдача, обмен денег · предлагать продукты и сервисы Сбера · консультировать клиентов по возникающим вопросам.   Работа в Сбере – это:   · стабильный оклад и социальная поддержка сотрудников · возможность выбрать удобный график работы · дополнительный доход ежемесячно · возможностью совмещать работу с другой занятостью и увлечениями · официальное оформление · расширенная пенсионная программа · бесплатная подписка СберПрайм+ и скидки на продукты компаний-партнеров · оплачиваемая мобильная связь: 150 минут и 3 ГБ интернета Сбермобайла · ипотека выгоднее на 4%.   Присоединяйся к команде Сбера!    АтмосфераРабота в Сбере –</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>https://hh.ru/vacancy/75668957?from=vacancy_search_list</t>
+          <t>https://hh.ru/vacancy/73871474?from=vacancy_search_list</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Специалист по приему и исполнению заказов</t>
+          <t>Старший клиентский менеджер</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>от 37000 до 43000 руб. на руки</t>
+          <t>от 34600 руб. до вычета налогов</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>В связи с открытием дополнительного филиала, в Компанию "Буряков" требуется специалист по приему и исполнению заказов. Обязанности: - Прием и обработка заказов от постоянных клиентов - Ведение учета в СРМ и 1С. - Подбор исполнителей из базы - Контроль и координация процесса исполнения заказов Требования: - Опыт работы на подобной должности желателен - Грамотная речь - Уверенные навыки работы с ПК - Опыт работы с СРМ и 1С - Коммуникабельность Условия: - График работы 5/2, с возможным переходом на график 2/2 - Можно без опыта работы, есть обучение - Заработная плата 2 раза в месяц: оклад (37000)+премия - Корпоративная связь - Возможность профессионального развития и карьерного роста  Ключевые навыкиТочность и внимательность к деталямПользователь ПКЗнание 1ССРМРабота в условиях многозадачностиУмение работать с людьмиУмение работать с клиентамиГрамотная речьЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопрос</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Точность и внимательность к деталям / Пользователь ПК / Знание 1С / СРМ / Работа в условиях многозадачности / Умение работать с людьми / Умение работать с клиентами / Грамотная речь / </t>
-        </is>
-      </c>
+          <t>Сбер — лучший работодатель России. У нас более 60 компаний экосистемы и 14 тысяч подразделений по всей стране. Мы ищем старшего менеджера по сопровождению клиентов. Его главная задача – помогать клиентам с оформлением продуктов и услуг Сбера и экосистемы, а также консультировать по возникающим вопросам. Эта вакансия для тех, кто хочет развивать навыки эффективных продаж и стоить карьеру в банковской сфере. Эта работа подойдет тебе если ты: · специалист со средним профессиональным, неполным высшим или высшим образованием · имеешь опыт работы в сфере продаж, обслуживания и консультирования клиентов от 6 месяцев · доброжелателен и готов помогать клиентам.   Тебе предстоит:   · предлагать продукты и услуги Сбера · консультировать клиентов по возникающим вопросам · помогать клиентам оформлять услуги и необходимые для них документы · совершать транзакционные операции в рамках оформления продаж и постпродажного сопровождения клиентов · вести базы клиентов.   Работа в Сбере – это:  · стабильный оклад и социальная поддержка сотрудников · официальное оформление с первого дня · расширенный ДМС с первого дня и льготное страхование для близких · корпоративное обучение в Виртуальной школе Сбера · бесплатная подписка СберПрайм+, скидки на продукты компаний-партнеров · корпоративная пенсионная программа · ипотека выгоднее на 4% для каждого сотрудника.   Присоединяйся к команде старших клиентских менеджеров Сбера!АтмосфераРабота в Сбере – это:Обучение за счет компании: онлайн курсы в Виртуальной школе Сбера, возможность получить новую квалификациюРеферальная программа для сотрудников: пригласи в команду знакомых профессионалов и получи свое вознаграждение до 100 тыс. рублейКурсы для будущих родителей, материальная поддержка молодых мам, детский отдых и подарки за счет компанииКорпоративная пенсионная программаДелай мир лучше со СберомЗадайте вопрос работодателюОн получит его с откликом на вакансиюГде располагается место работы?Какой график работы?Вакансия открыта?Какая оплата труда?Как с вами связаться?Другой вопросАдресИнжавиноПоказать на большой карте</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>